<commit_message>
updated MIDAS-F setup, RMSFEs, DM test
</commit_message>
<xml_diff>
--- a/Results/rmsfe/RMSFE_M.xlsx
+++ b/Results/rmsfe/RMSFE_M.xlsx
@@ -641,31 +641,31 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>0.67597</v>
+        <v>0.68</v>
       </c>
       <c r="C2" t="n">
-        <v>1.03639</v>
+        <v>1.04</v>
       </c>
       <c r="D2" t="n">
-        <v>1.01952</v>
+        <v>1.02</v>
       </c>
       <c r="E2" t="n">
-        <v>1.0125</v>
+        <v>1.06</v>
       </c>
       <c r="F2" t="n">
-        <v>1.00051</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>1.01101</v>
+        <v>1.01</v>
       </c>
       <c r="H2" t="n">
-        <v>0.99881</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>1.0235</v>
+        <v>1.02</v>
       </c>
       <c r="J2" t="n">
-        <v>0.96968</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="3">
@@ -673,31 +673,31 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>0.67597</v>
+        <v>0.68</v>
       </c>
       <c r="C3" t="n">
-        <v>1.03639</v>
+        <v>1.04</v>
       </c>
       <c r="D3" t="n">
-        <v>1.01991</v>
+        <v>1.02</v>
       </c>
       <c r="E3" t="n">
-        <v>1.01159</v>
+        <v>1.04</v>
       </c>
       <c r="F3" t="n">
-        <v>0.99525</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.99142</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="n">
-        <v>1.01687</v>
+        <v>1.02</v>
       </c>
       <c r="I3" t="n">
-        <v>1.0201</v>
+        <v>1.02</v>
       </c>
       <c r="J3" t="n">
-        <v>0.95226</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="4">
@@ -705,31 +705,31 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>0.67243</v>
+        <v>0.67</v>
       </c>
       <c r="C4" t="n">
-        <v>1.03435</v>
+        <v>1.03</v>
       </c>
       <c r="D4" t="n">
-        <v>1.012</v>
+        <v>1.01</v>
       </c>
       <c r="E4" t="n">
-        <v>1.01364</v>
+        <v>1.07</v>
       </c>
       <c r="F4" t="n">
-        <v>0.98842</v>
+        <v>0.99</v>
       </c>
       <c r="G4" t="n">
-        <v>0.99032</v>
+        <v>0.99</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9948</v>
+        <v>0.99</v>
       </c>
       <c r="I4" t="n">
-        <v>1.00957</v>
+        <v>1.01</v>
       </c>
       <c r="J4" t="n">
-        <v>0.92391</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="5">
@@ -737,31 +737,31 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>0.67243</v>
+        <v>0.67</v>
       </c>
       <c r="C5" t="n">
-        <v>1.03053</v>
+        <v>1.03</v>
       </c>
       <c r="D5" t="n">
-        <v>0.99947</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>1.01411</v>
+        <v>1.04</v>
       </c>
       <c r="F5" t="n">
-        <v>0.98449</v>
+        <v>0.98</v>
       </c>
       <c r="G5" t="n">
-        <v>0.98582</v>
+        <v>0.99</v>
       </c>
       <c r="H5" t="n">
-        <v>1.00274</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>1.01356</v>
+        <v>1.01</v>
       </c>
       <c r="J5" t="n">
-        <v>0.94394</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="6">
@@ -769,31 +769,31 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>0.67243</v>
+        <v>0.67</v>
       </c>
       <c r="C6" t="n">
-        <v>1.03053</v>
+        <v>1.03</v>
       </c>
       <c r="D6" t="n">
-        <v>0.99411</v>
+        <v>0.99</v>
       </c>
       <c r="E6" t="n">
-        <v>1.00249</v>
+        <v>1.03</v>
       </c>
       <c r="F6" t="n">
-        <v>0.98088</v>
+        <v>0.98</v>
       </c>
       <c r="G6" t="n">
-        <v>0.98878</v>
+        <v>0.99</v>
       </c>
       <c r="H6" t="n">
-        <v>0.99392</v>
+        <v>0.99</v>
       </c>
       <c r="I6" t="n">
-        <v>1.0047</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>0.94694</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="7">
@@ -801,31 +801,31 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>0.66929</v>
+        <v>0.67</v>
       </c>
       <c r="C7" t="n">
-        <v>1.02324</v>
+        <v>1.02</v>
       </c>
       <c r="D7" t="n">
-        <v>0.98852</v>
+        <v>0.99</v>
       </c>
       <c r="E7" t="n">
-        <v>0.97193</v>
+        <v>1.02</v>
       </c>
       <c r="F7" t="n">
-        <v>1.01394</v>
+        <v>1.01</v>
       </c>
       <c r="G7" t="n">
-        <v>1.0008</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9696</v>
+        <v>0.97</v>
       </c>
       <c r="I7" t="n">
-        <v>0.99185</v>
+        <v>0.99</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9224</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="8">
@@ -833,31 +833,31 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>0.66929</v>
+        <v>0.67</v>
       </c>
       <c r="C8" t="n">
-        <v>1.01113</v>
+        <v>1.01</v>
       </c>
       <c r="D8" t="n">
-        <v>0.98317</v>
+        <v>0.98</v>
       </c>
       <c r="E8" t="n">
-        <v>0.97389</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.94295</v>
+        <v>0.94</v>
       </c>
       <c r="G8" t="n">
-        <v>0.95193</v>
+        <v>0.95</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9495</v>
+        <v>0.95</v>
       </c>
       <c r="I8" t="n">
-        <v>0.99026</v>
+        <v>0.99</v>
       </c>
       <c r="J8" t="n">
-        <v>0.91486</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="9">
@@ -865,31 +865,31 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>0.66929</v>
+        <v>0.67</v>
       </c>
       <c r="C9" t="n">
-        <v>1.01113</v>
+        <v>1.01</v>
       </c>
       <c r="D9" t="n">
-        <v>0.95369</v>
+        <v>0.95</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9544</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.93315</v>
+        <v>0.93</v>
       </c>
       <c r="G9" t="n">
-        <v>0.91881</v>
+        <v>0.92</v>
       </c>
       <c r="H9" t="n">
-        <v>0.92776</v>
+        <v>0.93</v>
       </c>
       <c r="I9" t="n">
-        <v>0.97091</v>
+        <v>0.97</v>
       </c>
       <c r="J9" t="n">
-        <v>0.89997</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10">
@@ -897,31 +897,31 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>0.66737</v>
+        <v>0.67</v>
       </c>
       <c r="C10" t="n">
-        <v>0.95787</v>
+        <v>0.96</v>
       </c>
       <c r="D10" t="n">
-        <v>0.87607</v>
+        <v>0.88</v>
       </c>
       <c r="E10" t="n">
-        <v>0.92908</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.86782</v>
+        <v>0.87</v>
       </c>
       <c r="G10" t="n">
-        <v>0.86886</v>
+        <v>0.87</v>
       </c>
       <c r="H10" t="n">
-        <v>0.90392</v>
+        <v>0.9</v>
       </c>
       <c r="I10" t="n">
-        <v>0.93718</v>
+        <v>0.94</v>
       </c>
       <c r="J10" t="n">
-        <v>0.8793</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="11">
@@ -929,31 +929,31 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>0.66737</v>
+        <v>0.67</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9999</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0.82932</v>
+        <v>0.83</v>
       </c>
       <c r="E11" t="n">
-        <v>0.97173</v>
+        <v>0.97</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8416</v>
+        <v>0.84</v>
       </c>
       <c r="G11" t="n">
-        <v>0.85562</v>
+        <v>0.86</v>
       </c>
       <c r="H11" t="n">
-        <v>0.90845</v>
+        <v>0.91</v>
       </c>
       <c r="I11" t="n">
-        <v>0.96066</v>
+        <v>0.96</v>
       </c>
       <c r="J11" t="n">
-        <v>0.88674</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="12">
@@ -961,31 +961,31 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>0.66737</v>
+        <v>0.67</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9999</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.78718</v>
+        <v>0.79</v>
       </c>
       <c r="E12" t="n">
-        <v>0.98331</v>
+        <v>0.97</v>
       </c>
       <c r="F12" t="n">
-        <v>0.82319</v>
+        <v>0.82</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8669</v>
+        <v>0.87</v>
       </c>
       <c r="H12" t="n">
-        <v>0.90298</v>
+        <v>0.9</v>
       </c>
       <c r="I12" t="n">
-        <v>0.95914</v>
+        <v>0.96</v>
       </c>
       <c r="J12" t="n">
-        <v>0.8774</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="13">
@@ -993,31 +993,31 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>0.53472</v>
+        <v>0.53</v>
       </c>
       <c r="C13" t="n">
-        <v>1.05687</v>
+        <v>1.06</v>
       </c>
       <c r="D13" t="n">
-        <v>1.00489</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>1.03223</v>
+        <v>1.09</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9957</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>1.02835</v>
+        <v>1.03</v>
       </c>
       <c r="H13" t="n">
-        <v>0.99847</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>1.05044</v>
+        <v>1.05</v>
       </c>
       <c r="J13" t="n">
-        <v>1.03474</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="14">
@@ -1025,31 +1025,31 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>0.53472</v>
+        <v>0.53</v>
       </c>
       <c r="C14" t="n">
-        <v>1.05687</v>
+        <v>1.06</v>
       </c>
       <c r="D14" t="n">
-        <v>1.00333</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>1.02309</v>
+        <v>1.06</v>
       </c>
       <c r="F14" t="n">
-        <v>1.00523</v>
+        <v>1.01</v>
       </c>
       <c r="G14" t="n">
-        <v>0.99098</v>
+        <v>0.99</v>
       </c>
       <c r="H14" t="n">
-        <v>1.04523</v>
+        <v>1.05</v>
       </c>
       <c r="I14" t="n">
-        <v>1.02116</v>
+        <v>1.02</v>
       </c>
       <c r="J14" t="n">
-        <v>0.9989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1057,31 +1057,31 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>0.53164</v>
+        <v>0.53</v>
       </c>
       <c r="C15" t="n">
-        <v>1.05269</v>
+        <v>1.05</v>
       </c>
       <c r="D15" t="n">
-        <v>0.98948</v>
+        <v>0.99</v>
       </c>
       <c r="E15" t="n">
-        <v>1.01605</v>
+        <v>1.06</v>
       </c>
       <c r="F15" t="n">
-        <v>0.94906</v>
+        <v>0.95</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9544</v>
+        <v>0.95</v>
       </c>
       <c r="H15" t="n">
-        <v>0.99579</v>
+        <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.97757</v>
+        <v>0.98</v>
       </c>
       <c r="J15" t="n">
-        <v>0.9223</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="16">
@@ -1089,31 +1089,31 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>0.53164</v>
+        <v>0.53</v>
       </c>
       <c r="C16" t="n">
-        <v>1.04789</v>
+        <v>1.05</v>
       </c>
       <c r="D16" t="n">
-        <v>0.97061</v>
+        <v>0.97</v>
       </c>
       <c r="E16" t="n">
-        <v>1.0269</v>
+        <v>1.05</v>
       </c>
       <c r="F16" t="n">
-        <v>1.02861</v>
+        <v>1.03</v>
       </c>
       <c r="G16" t="n">
-        <v>1.02111</v>
+        <v>1.02</v>
       </c>
       <c r="H16" t="n">
-        <v>1.02407</v>
+        <v>1.02</v>
       </c>
       <c r="I16" t="n">
-        <v>1.02402</v>
+        <v>1.02</v>
       </c>
       <c r="J16" t="n">
-        <v>0.96497</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="17">
@@ -1121,31 +1121,31 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>0.53164</v>
+        <v>0.53</v>
       </c>
       <c r="C17" t="n">
-        <v>1.04789</v>
+        <v>1.05</v>
       </c>
       <c r="D17" t="n">
-        <v>0.98046</v>
+        <v>0.98</v>
       </c>
       <c r="E17" t="n">
-        <v>1.02447</v>
+        <v>1.06</v>
       </c>
       <c r="F17" t="n">
-        <v>1.00326</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>1.0065</v>
+        <v>1.01</v>
       </c>
       <c r="H17" t="n">
-        <v>1.0018</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>0.99878</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>0.95347</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="18">
@@ -1153,31 +1153,31 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>0.52808</v>
+        <v>0.53</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0419</v>
+        <v>1.04</v>
       </c>
       <c r="D18" t="n">
-        <v>0.98328</v>
+        <v>0.98</v>
       </c>
       <c r="E18" t="n">
-        <v>1.01227</v>
+        <v>1.05</v>
       </c>
       <c r="F18" t="n">
-        <v>1.03516</v>
+        <v>1.04</v>
       </c>
       <c r="G18" t="n">
-        <v>0.98609</v>
+        <v>0.99</v>
       </c>
       <c r="H18" t="n">
-        <v>0.97847</v>
+        <v>0.98</v>
       </c>
       <c r="I18" t="n">
-        <v>0.98268</v>
+        <v>0.98</v>
       </c>
       <c r="J18" t="n">
-        <v>0.92332</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="19">
@@ -1185,31 +1185,31 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>0.52808</v>
+        <v>0.53</v>
       </c>
       <c r="C19" t="n">
-        <v>1.039</v>
+        <v>1.04</v>
       </c>
       <c r="D19" t="n">
-        <v>0.97928</v>
+        <v>0.98</v>
       </c>
       <c r="E19" t="n">
-        <v>1.01905</v>
+        <v>1.02</v>
       </c>
       <c r="F19" t="n">
-        <v>1.00155</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>1.0055</v>
+        <v>1.01</v>
       </c>
       <c r="H19" t="n">
-        <v>0.96866</v>
+        <v>0.97</v>
       </c>
       <c r="I19" t="n">
-        <v>1.02956</v>
+        <v>1.03</v>
       </c>
       <c r="J19" t="n">
-        <v>0.94205</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="20">
@@ -1217,31 +1217,31 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>0.52808</v>
+        <v>0.53</v>
       </c>
       <c r="C20" t="n">
-        <v>1.039</v>
+        <v>1.04</v>
       </c>
       <c r="D20" t="n">
-        <v>0.9776</v>
+        <v>0.98</v>
       </c>
       <c r="E20" t="n">
-        <v>1.01831</v>
+        <v>1.04</v>
       </c>
       <c r="F20" t="n">
-        <v>1.0051</v>
+        <v>1.01</v>
       </c>
       <c r="G20" t="n">
-        <v>0.994</v>
+        <v>0.99</v>
       </c>
       <c r="H20" t="n">
-        <v>0.95225</v>
+        <v>0.95</v>
       </c>
       <c r="I20" t="n">
-        <v>1.01649</v>
+        <v>1.02</v>
       </c>
       <c r="J20" t="n">
-        <v>0.91939</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="21">
@@ -1249,31 +1249,31 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>0.52563</v>
+        <v>0.53</v>
       </c>
       <c r="C21" t="n">
-        <v>1.01627</v>
+        <v>1.02</v>
       </c>
       <c r="D21" t="n">
-        <v>0.95297</v>
+        <v>0.95</v>
       </c>
       <c r="E21" t="n">
-        <v>1.01378</v>
+        <v>1.04</v>
       </c>
       <c r="F21" t="n">
-        <v>0.99195</v>
+        <v>0.99</v>
       </c>
       <c r="G21" t="n">
-        <v>0.9866</v>
+        <v>0.99</v>
       </c>
       <c r="H21" t="n">
-        <v>0.96525</v>
+        <v>0.97</v>
       </c>
       <c r="I21" t="n">
-        <v>0.99964</v>
+        <v>1</v>
       </c>
       <c r="J21" t="n">
-        <v>0.91183</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="22">
@@ -1281,31 +1281,31 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>0.52563</v>
+        <v>0.53</v>
       </c>
       <c r="C22" t="n">
-        <v>1.03295</v>
+        <v>1.03</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9244</v>
+        <v>0.92</v>
       </c>
       <c r="E22" t="n">
-        <v>1.01872</v>
+        <v>1.03</v>
       </c>
       <c r="F22" t="n">
-        <v>0.99425</v>
+        <v>0.99</v>
       </c>
       <c r="G22" t="n">
-        <v>0.97621</v>
+        <v>0.98</v>
       </c>
       <c r="H22" t="n">
-        <v>0.98668</v>
+        <v>0.99</v>
       </c>
       <c r="I22" t="n">
-        <v>1.03251</v>
+        <v>1.03</v>
       </c>
       <c r="J22" t="n">
-        <v>0.96644</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="23">
@@ -1313,31 +1313,31 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>0.52563</v>
+        <v>0.53</v>
       </c>
       <c r="C23" t="n">
-        <v>1.03295</v>
+        <v>1.03</v>
       </c>
       <c r="D23" t="n">
-        <v>0.88109</v>
+        <v>0.88</v>
       </c>
       <c r="E23" t="n">
-        <v>1.00468</v>
+        <v>1.03</v>
       </c>
       <c r="F23" t="n">
-        <v>0.98426</v>
+        <v>0.98</v>
       </c>
       <c r="G23" t="n">
-        <v>0.97988</v>
+        <v>0.98</v>
       </c>
       <c r="H23" t="n">
-        <v>0.96958</v>
+        <v>0.97</v>
       </c>
       <c r="I23" t="n">
-        <v>1.02418</v>
+        <v>1.02</v>
       </c>
       <c r="J23" t="n">
-        <v>0.93664</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="24">
@@ -1345,31 +1345,31 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>1.3635</v>
+        <v>1.36</v>
       </c>
       <c r="C24" t="n">
-        <v>1.02218</v>
+        <v>1.02</v>
       </c>
       <c r="D24" t="n">
-        <v>1.02332</v>
+        <v>1.02</v>
       </c>
       <c r="E24" t="n">
-        <v>0.99934</v>
+        <v>0.97</v>
       </c>
       <c r="F24" t="n">
-        <v>0.99556</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>0.99304</v>
+        <v>0.99</v>
       </c>
       <c r="H24" t="n">
-        <v>0.98894</v>
+        <v>0.99</v>
       </c>
       <c r="I24" t="n">
-        <v>0.98843</v>
+        <v>0.99</v>
       </c>
       <c r="J24" t="n">
-        <v>0.92119</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="25">
@@ -1377,31 +1377,31 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>1.3635</v>
+        <v>1.36</v>
       </c>
       <c r="C25" t="n">
-        <v>1.02218</v>
+        <v>1.02</v>
       </c>
       <c r="D25" t="n">
-        <v>1.02358</v>
+        <v>1.02</v>
       </c>
       <c r="E25" t="n">
-        <v>0.99717</v>
+        <v>0.97</v>
       </c>
       <c r="F25" t="n">
-        <v>0.97295</v>
+        <v>0.97</v>
       </c>
       <c r="G25" t="n">
-        <v>0.97184</v>
+        <v>0.97</v>
       </c>
       <c r="H25" t="n">
-        <v>0.99076</v>
+        <v>0.99</v>
       </c>
       <c r="I25" t="n">
-        <v>0.99576</v>
+        <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>0.90409</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="26">
@@ -1409,31 +1409,31 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>1.35686</v>
+        <v>1.36</v>
       </c>
       <c r="C26" t="n">
-        <v>1.02785</v>
+        <v>1.03</v>
       </c>
       <c r="D26" t="n">
-        <v>1.02195</v>
+        <v>1.02</v>
       </c>
       <c r="E26" t="n">
-        <v>1.00364</v>
+        <v>0.98</v>
       </c>
       <c r="F26" t="n">
-        <v>0.98262</v>
+        <v>0.98</v>
       </c>
       <c r="G26" t="n">
-        <v>0.9952</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
-        <v>0.98554</v>
+        <v>0.99</v>
       </c>
       <c r="I26" t="n">
-        <v>1.00709</v>
+        <v>1.01</v>
       </c>
       <c r="J26" t="n">
-        <v>0.90838</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="27">
@@ -1441,31 +1441,31 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>1.35686</v>
+        <v>1.36</v>
       </c>
       <c r="C27" t="n">
-        <v>1.02072</v>
+        <v>1.02</v>
       </c>
       <c r="D27" t="n">
-        <v>1.01824</v>
+        <v>1.02</v>
       </c>
       <c r="E27" t="n">
-        <v>1.00663</v>
+        <v>0.99</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9506</v>
+        <v>0.95</v>
       </c>
       <c r="G27" t="n">
-        <v>0.96607</v>
+        <v>0.97</v>
       </c>
       <c r="H27" t="n">
-        <v>0.99192</v>
+        <v>0.99</v>
       </c>
       <c r="I27" t="n">
-        <v>1.00083</v>
+        <v>1</v>
       </c>
       <c r="J27" t="n">
-        <v>0.93635</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="28">
@@ -1473,31 +1473,31 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>1.35686</v>
+        <v>1.36</v>
       </c>
       <c r="C28" t="n">
-        <v>1.02072</v>
+        <v>1.02</v>
       </c>
       <c r="D28" t="n">
-        <v>1.01256</v>
+        <v>1.01</v>
       </c>
       <c r="E28" t="n">
-        <v>0.99235</v>
+        <v>0.99</v>
       </c>
       <c r="F28" t="n">
-        <v>0.95454</v>
+        <v>0.95</v>
       </c>
       <c r="G28" t="n">
-        <v>0.95265</v>
+        <v>0.95</v>
       </c>
       <c r="H28" t="n">
-        <v>0.99045</v>
+        <v>0.99</v>
       </c>
       <c r="I28" t="n">
-        <v>1.002</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>0.94974</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="29">
@@ -1505,31 +1505,31 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>1.35328</v>
+        <v>1.35</v>
       </c>
       <c r="C29" t="n">
-        <v>1.02381</v>
+        <v>1.02</v>
       </c>
       <c r="D29" t="n">
-        <v>0.99149</v>
+        <v>0.99</v>
       </c>
       <c r="E29" t="n">
-        <v>0.93983</v>
+        <v>0.97</v>
       </c>
       <c r="F29" t="n">
-        <v>0.98446</v>
+        <v>0.98</v>
       </c>
       <c r="G29" t="n">
-        <v>0.96763</v>
+        <v>0.97</v>
       </c>
       <c r="H29" t="n">
-        <v>0.96314</v>
+        <v>0.96</v>
       </c>
       <c r="I29" t="n">
-        <v>0.98735</v>
+        <v>0.99</v>
       </c>
       <c r="J29" t="n">
-        <v>0.92384</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="30">
@@ -1537,31 +1537,31 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>1.35328</v>
+        <v>1.35</v>
       </c>
       <c r="C30" t="n">
-        <v>1.00762</v>
+        <v>1.01</v>
       </c>
       <c r="D30" t="n">
-        <v>0.98605</v>
+        <v>0.99</v>
       </c>
       <c r="E30" t="n">
-        <v>0.93373</v>
+        <v>0.95</v>
       </c>
       <c r="F30" t="n">
-        <v>0.89837</v>
+        <v>0.9</v>
       </c>
       <c r="G30" t="n">
-        <v>0.91946</v>
+        <v>0.92</v>
       </c>
       <c r="H30" t="n">
-        <v>0.94537</v>
+        <v>0.95</v>
       </c>
       <c r="I30" t="n">
-        <v>0.95818</v>
+        <v>0.96</v>
       </c>
       <c r="J30" t="n">
-        <v>0.90373</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="31">
@@ -1569,31 +1569,31 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1.35328</v>
+        <v>1.35</v>
       </c>
       <c r="C31" t="n">
-        <v>1.00762</v>
+        <v>1.01</v>
       </c>
       <c r="D31" t="n">
-        <v>0.93136</v>
+        <v>0.93</v>
       </c>
       <c r="E31" t="n">
-        <v>0.89156</v>
+        <v>0.95</v>
       </c>
       <c r="F31" t="n">
-        <v>0.7801</v>
+        <v>0.78</v>
       </c>
       <c r="G31" t="n">
-        <v>0.79422</v>
+        <v>0.79</v>
       </c>
       <c r="H31" t="n">
-        <v>0.90992</v>
+        <v>0.91</v>
       </c>
       <c r="I31" t="n">
-        <v>0.92733</v>
+        <v>0.93</v>
       </c>
       <c r="J31" t="n">
-        <v>0.88218</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="32">
@@ -1601,31 +1601,31 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1.35223</v>
+        <v>1.35</v>
       </c>
       <c r="C32" t="n">
-        <v>0.93163</v>
+        <v>0.93</v>
       </c>
       <c r="D32" t="n">
-        <v>0.78434</v>
+        <v>0.78</v>
       </c>
       <c r="E32" t="n">
-        <v>0.83526</v>
+        <v>0.94</v>
       </c>
       <c r="F32" t="n">
-        <v>0.68529</v>
+        <v>0.69</v>
       </c>
       <c r="G32" t="n">
-        <v>0.70585</v>
+        <v>0.71</v>
       </c>
       <c r="H32" t="n">
-        <v>0.85094</v>
+        <v>0.85</v>
       </c>
       <c r="I32" t="n">
-        <v>0.87363</v>
+        <v>0.87</v>
       </c>
       <c r="J32" t="n">
-        <v>0.85096</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="33">
@@ -1633,31 +1633,31 @@
         <v>41</v>
       </c>
       <c r="B33" t="n">
-        <v>1.35223</v>
+        <v>1.35</v>
       </c>
       <c r="C33" t="n">
-        <v>0.98555</v>
+        <v>0.99</v>
       </c>
       <c r="D33" t="n">
-        <v>0.70981</v>
+        <v>0.71</v>
       </c>
       <c r="E33" t="n">
-        <v>0.91674</v>
+        <v>0.88</v>
       </c>
       <c r="F33" t="n">
-        <v>0.65205</v>
+        <v>0.65</v>
       </c>
       <c r="G33" t="n">
-        <v>0.7224</v>
+        <v>0.72</v>
       </c>
       <c r="H33" t="n">
-        <v>0.83322</v>
+        <v>0.83</v>
       </c>
       <c r="I33" t="n">
-        <v>0.90429</v>
+        <v>0.9</v>
       </c>
       <c r="J33" t="n">
-        <v>0.82149</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="34">
@@ -1665,31 +1665,31 @@
         <v>42</v>
       </c>
       <c r="B34" t="n">
-        <v>1.35223</v>
+        <v>1.35</v>
       </c>
       <c r="C34" t="n">
-        <v>0.98555</v>
+        <v>0.99</v>
       </c>
       <c r="D34" t="n">
-        <v>0.65765</v>
+        <v>0.66</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9592</v>
+        <v>0.9</v>
       </c>
       <c r="F34" t="n">
-        <v>0.64759</v>
+        <v>0.65</v>
       </c>
       <c r="G34" t="n">
-        <v>0.68505</v>
+        <v>0.69</v>
       </c>
       <c r="H34" t="n">
-        <v>0.83408</v>
+        <v>0.83</v>
       </c>
       <c r="I34" t="n">
-        <v>0.90574</v>
+        <v>0.91</v>
       </c>
       <c r="J34" t="n">
-        <v>0.82921</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="35">
@@ -1697,31 +1697,31 @@
         <v>43</v>
       </c>
       <c r="B35" t="n">
-        <v>0.52221</v>
+        <v>0.52</v>
       </c>
       <c r="C35" t="n">
-        <v>1.02815</v>
+        <v>1.03</v>
       </c>
       <c r="D35" t="n">
-        <v>1.04116</v>
+        <v>1.04</v>
       </c>
       <c r="E35" t="n">
-        <v>1.00313</v>
+        <v>1.19</v>
       </c>
       <c r="F35" t="n">
-        <v>1.02383</v>
+        <v>1.02</v>
       </c>
       <c r="G35" t="n">
-        <v>1.01952</v>
+        <v>1.02</v>
       </c>
       <c r="H35" t="n">
-        <v>1.02514</v>
+        <v>1.03</v>
       </c>
       <c r="I35" t="n">
-        <v>1.05401</v>
+        <v>1.05</v>
       </c>
       <c r="J35" t="n">
-        <v>0.94636</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="36">
@@ -1729,31 +1729,31 @@
         <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>0.52221</v>
+        <v>0.52</v>
       </c>
       <c r="C36" t="n">
-        <v>1.02815</v>
+        <v>1.03</v>
       </c>
       <c r="D36" t="n">
-        <v>1.04601</v>
+        <v>1.05</v>
       </c>
       <c r="E36" t="n">
-        <v>1.02389</v>
+        <v>1.17</v>
       </c>
       <c r="F36" t="n">
-        <v>1.03078</v>
+        <v>1.03</v>
       </c>
       <c r="G36" t="n">
-        <v>1.04225</v>
+        <v>1.04</v>
       </c>
       <c r="H36" t="n">
-        <v>1.02165</v>
+        <v>1.02</v>
       </c>
       <c r="I36" t="n">
-        <v>1.07949</v>
+        <v>1.08</v>
       </c>
       <c r="J36" t="n">
-        <v>0.97091</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="37">
@@ -1761,31 +1761,31 @@
         <v>45</v>
       </c>
       <c r="B37" t="n">
-        <v>0.5196</v>
+        <v>0.52</v>
       </c>
       <c r="C37" t="n">
-        <v>1.01056</v>
+        <v>1.01</v>
       </c>
       <c r="D37" t="n">
-        <v>1.03425</v>
+        <v>1.03</v>
       </c>
       <c r="E37" t="n">
-        <v>1.03441</v>
+        <v>1.28</v>
       </c>
       <c r="F37" t="n">
-        <v>1.08381</v>
+        <v>1.08</v>
       </c>
       <c r="G37" t="n">
-        <v>1.05284</v>
+        <v>1.05</v>
       </c>
       <c r="H37" t="n">
-        <v>1.01674</v>
+        <v>1.02</v>
       </c>
       <c r="I37" t="n">
-        <v>1.08259</v>
+        <v>1.08</v>
       </c>
       <c r="J37" t="n">
-        <v>0.96708</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="38">
@@ -1793,31 +1793,31 @@
         <v>46</v>
       </c>
       <c r="B38" t="n">
-        <v>0.5196</v>
+        <v>0.52</v>
       </c>
       <c r="C38" t="n">
-        <v>1.01778</v>
+        <v>1.02</v>
       </c>
       <c r="D38" t="n">
-        <v>1.01178</v>
+        <v>1.01</v>
       </c>
       <c r="E38" t="n">
-        <v>1.00547</v>
+        <v>1.13</v>
       </c>
       <c r="F38" t="n">
-        <v>0.97336</v>
+        <v>0.97</v>
       </c>
       <c r="G38" t="n">
-        <v>0.95823</v>
+        <v>0.96</v>
       </c>
       <c r="H38" t="n">
-        <v>0.98364</v>
+        <v>0.98</v>
       </c>
       <c r="I38" t="n">
-        <v>1.02383</v>
+        <v>1.02</v>
       </c>
       <c r="J38" t="n">
-        <v>0.91681</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="39">
@@ -1825,31 +1825,31 @@
         <v>47</v>
       </c>
       <c r="B39" t="n">
-        <v>0.5196</v>
+        <v>0.52</v>
       </c>
       <c r="C39" t="n">
-        <v>1.01778</v>
+        <v>1.02</v>
       </c>
       <c r="D39" t="n">
-        <v>0.97452</v>
+        <v>0.97</v>
       </c>
       <c r="E39" t="n">
-        <v>0.9801</v>
+        <v>1.06</v>
       </c>
       <c r="F39" t="n">
-        <v>0.99962</v>
+        <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>1.04175</v>
+        <v>1.04</v>
       </c>
       <c r="H39" t="n">
-        <v>0.98565</v>
+        <v>0.99</v>
       </c>
       <c r="I39" t="n">
-        <v>1.02456</v>
+        <v>1.02</v>
       </c>
       <c r="J39" t="n">
-        <v>0.92487</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="40">
@@ -1857,31 +1857,31 @@
         <v>48</v>
       </c>
       <c r="B40" t="n">
-        <v>0.51667</v>
+        <v>0.52</v>
       </c>
       <c r="C40" t="n">
-        <v>0.97957</v>
+        <v>0.98</v>
       </c>
       <c r="D40" t="n">
-        <v>0.99205</v>
+        <v>0.99</v>
       </c>
       <c r="E40" t="n">
-        <v>0.96558</v>
+        <v>1.07</v>
       </c>
       <c r="F40" t="n">
-        <v>1.04369</v>
+        <v>1.04</v>
       </c>
       <c r="G40" t="n">
-        <v>1.11313</v>
+        <v>1.11</v>
       </c>
       <c r="H40" t="n">
-        <v>0.96719</v>
+        <v>0.97</v>
       </c>
       <c r="I40" t="n">
-        <v>1.02328</v>
+        <v>1.02</v>
       </c>
       <c r="J40" t="n">
-        <v>0.91656</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="41">
@@ -1889,31 +1889,31 @@
         <v>49</v>
       </c>
       <c r="B41" t="n">
-        <v>0.51667</v>
+        <v>0.52</v>
       </c>
       <c r="C41" t="n">
-        <v>0.95709</v>
+        <v>0.96</v>
       </c>
       <c r="D41" t="n">
-        <v>0.98401</v>
+        <v>0.98</v>
       </c>
       <c r="E41" t="n">
-        <v>0.97708</v>
+        <v>1.06</v>
       </c>
       <c r="F41" t="n">
-        <v>0.92606</v>
+        <v>0.93</v>
       </c>
       <c r="G41" t="n">
-        <v>0.91533</v>
+        <v>0.92</v>
       </c>
       <c r="H41" t="n">
-        <v>0.91752</v>
+        <v>0.92</v>
       </c>
       <c r="I41" t="n">
-        <v>0.9863</v>
+        <v>0.99</v>
       </c>
       <c r="J41" t="n">
-        <v>0.88328</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="42">
@@ -1921,31 +1921,31 @@
         <v>50</v>
       </c>
       <c r="B42" t="n">
-        <v>0.51667</v>
+        <v>0.52</v>
       </c>
       <c r="C42" t="n">
-        <v>0.95709</v>
+        <v>0.96</v>
       </c>
       <c r="D42" t="n">
-        <v>0.95928</v>
+        <v>0.96</v>
       </c>
       <c r="E42" t="n">
-        <v>0.97095</v>
+        <v>1.06</v>
       </c>
       <c r="F42" t="n">
-        <v>1.12323</v>
+        <v>1.12</v>
       </c>
       <c r="G42" t="n">
-        <v>1.04689</v>
+        <v>1.05</v>
       </c>
       <c r="H42" t="n">
-        <v>0.92028</v>
+        <v>0.92</v>
       </c>
       <c r="I42" t="n">
-        <v>0.9818</v>
+        <v>0.98</v>
       </c>
       <c r="J42" t="n">
-        <v>0.90373</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="43">
@@ -1953,31 +1953,31 @@
         <v>51</v>
       </c>
       <c r="B43" t="n">
-        <v>0.51436</v>
+        <v>0.51</v>
       </c>
       <c r="C43" t="n">
-        <v>0.89314</v>
+        <v>0.89</v>
       </c>
       <c r="D43" t="n">
-        <v>0.93113</v>
+        <v>0.93</v>
       </c>
       <c r="E43" t="n">
-        <v>0.97248</v>
+        <v>1.03</v>
       </c>
       <c r="F43" t="n">
-        <v>1.00304</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>0.98151</v>
+        <v>0.98</v>
       </c>
       <c r="H43" t="n">
-        <v>0.90267</v>
+        <v>0.9</v>
       </c>
       <c r="I43" t="n">
-        <v>0.95986</v>
+        <v>0.96</v>
       </c>
       <c r="J43" t="n">
-        <v>0.88133</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="44">
@@ -1985,31 +1985,31 @@
         <v>52</v>
       </c>
       <c r="B44" t="n">
-        <v>0.51436</v>
+        <v>0.51</v>
       </c>
       <c r="C44" t="n">
-        <v>0.96381</v>
+        <v>0.96</v>
       </c>
       <c r="D44" t="n">
-        <v>0.90266</v>
+        <v>0.9</v>
       </c>
       <c r="E44" t="n">
-        <v>1.0086</v>
+        <v>1.06</v>
       </c>
       <c r="F44" t="n">
-        <v>0.92312</v>
+        <v>0.92</v>
       </c>
       <c r="G44" t="n">
-        <v>0.90045</v>
+        <v>0.9</v>
       </c>
       <c r="H44" t="n">
-        <v>0.92259</v>
+        <v>0.92</v>
       </c>
       <c r="I44" t="n">
-        <v>0.94371</v>
+        <v>0.94</v>
       </c>
       <c r="J44" t="n">
-        <v>0.87241</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="45">
@@ -2017,31 +2017,31 @@
         <v>53</v>
       </c>
       <c r="B45" t="n">
-        <v>0.51436</v>
+        <v>0.51</v>
       </c>
       <c r="C45" t="n">
-        <v>0.96381</v>
+        <v>0.96</v>
       </c>
       <c r="D45" t="n">
-        <v>0.88164</v>
+        <v>0.88</v>
       </c>
       <c r="E45" t="n">
-        <v>0.99959</v>
+        <v>1.01</v>
       </c>
       <c r="F45" t="n">
-        <v>0.85506</v>
+        <v>0.86</v>
       </c>
       <c r="G45" t="n">
-        <v>1.02454</v>
+        <v>1.02</v>
       </c>
       <c r="H45" t="n">
-        <v>0.92871</v>
+        <v>0.93</v>
       </c>
       <c r="I45" t="n">
-        <v>0.95077</v>
+        <v>0.95</v>
       </c>
       <c r="J45" t="n">
-        <v>0.86861</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="46">
@@ -2049,31 +2049,31 @@
         <v>54</v>
       </c>
       <c r="B46" t="n">
-        <v>1.21478</v>
+        <v>1.21</v>
       </c>
       <c r="C46" t="n">
-        <v>1.0314</v>
+        <v>1.03</v>
       </c>
       <c r="D46" t="n">
-        <v>0.99516</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>0.9725</v>
+        <v>1.03</v>
       </c>
       <c r="F46" t="n">
-        <v>0.98811</v>
+        <v>0.99</v>
       </c>
       <c r="G46" t="n">
-        <v>0.9919</v>
+        <v>0.99</v>
       </c>
       <c r="H46" t="n">
-        <v>0.97195</v>
+        <v>0.97</v>
       </c>
       <c r="I46" t="n">
-        <v>0.99999</v>
+        <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>0.92286</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="47">
@@ -2081,31 +2081,31 @@
         <v>55</v>
       </c>
       <c r="B47" t="n">
-        <v>1.21478</v>
+        <v>1.21</v>
       </c>
       <c r="C47" t="n">
-        <v>1.0314</v>
+        <v>1.03</v>
       </c>
       <c r="D47" t="n">
-        <v>0.99113</v>
+        <v>0.99</v>
       </c>
       <c r="E47" t="n">
-        <v>0.9703</v>
+        <v>1.01</v>
       </c>
       <c r="F47" t="n">
-        <v>0.96167</v>
+        <v>0.96</v>
       </c>
       <c r="G47" t="n">
-        <v>0.9706</v>
+        <v>0.97</v>
       </c>
       <c r="H47" t="n">
-        <v>0.99263</v>
+        <v>0.99</v>
       </c>
       <c r="I47" t="n">
-        <v>1.00556</v>
+        <v>1.01</v>
       </c>
       <c r="J47" t="n">
-        <v>0.92426</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="48">
@@ -2113,31 +2113,31 @@
         <v>56</v>
       </c>
       <c r="B48" t="n">
-        <v>1.20928</v>
+        <v>1.21</v>
       </c>
       <c r="C48" t="n">
-        <v>1.03145</v>
+        <v>1.03</v>
       </c>
       <c r="D48" t="n">
-        <v>0.96792</v>
+        <v>0.97</v>
       </c>
       <c r="E48" t="n">
-        <v>0.96442</v>
+        <v>1.04</v>
       </c>
       <c r="F48" t="n">
-        <v>0.96715</v>
+        <v>0.97</v>
       </c>
       <c r="G48" t="n">
-        <v>0.9681</v>
+        <v>0.97</v>
       </c>
       <c r="H48" t="n">
-        <v>0.96871</v>
+        <v>0.97</v>
       </c>
       <c r="I48" t="n">
-        <v>0.9964</v>
+        <v>1</v>
       </c>
       <c r="J48" t="n">
-        <v>0.90993</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="49">
@@ -2145,31 +2145,31 @@
         <v>57</v>
       </c>
       <c r="B49" t="n">
-        <v>1.20928</v>
+        <v>1.21</v>
       </c>
       <c r="C49" t="n">
-        <v>1.02789</v>
+        <v>1.03</v>
       </c>
       <c r="D49" t="n">
-        <v>0.94752</v>
+        <v>0.95</v>
       </c>
       <c r="E49" t="n">
-        <v>0.97849</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>0.89934</v>
+        <v>0.9</v>
       </c>
       <c r="G49" t="n">
-        <v>0.91872</v>
+        <v>0.92</v>
       </c>
       <c r="H49" t="n">
-        <v>0.96539</v>
+        <v>0.97</v>
       </c>
       <c r="I49" t="n">
-        <v>0.98984</v>
+        <v>0.99</v>
       </c>
       <c r="J49" t="n">
-        <v>0.90911</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="50">
@@ -2177,31 +2177,31 @@
         <v>58</v>
       </c>
       <c r="B50" t="n">
-        <v>1.20928</v>
+        <v>1.21</v>
       </c>
       <c r="C50" t="n">
-        <v>1.02789</v>
+        <v>1.03</v>
       </c>
       <c r="D50" t="n">
-        <v>0.94107</v>
+        <v>0.94</v>
       </c>
       <c r="E50" t="n">
-        <v>0.9577</v>
+        <v>0.98</v>
       </c>
       <c r="F50" t="n">
-        <v>0.87532</v>
+        <v>0.88</v>
       </c>
       <c r="G50" t="n">
-        <v>0.89507</v>
+        <v>0.9</v>
       </c>
       <c r="H50" t="n">
-        <v>0.93965</v>
+        <v>0.94</v>
       </c>
       <c r="I50" t="n">
-        <v>0.9833</v>
+        <v>0.98</v>
       </c>
       <c r="J50" t="n">
-        <v>0.9203</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="51">
@@ -2209,31 +2209,31 @@
         <v>59</v>
       </c>
       <c r="B51" t="n">
-        <v>1.20444</v>
+        <v>1.2</v>
       </c>
       <c r="C51" t="n">
-        <v>1.01661</v>
+        <v>1.02</v>
       </c>
       <c r="D51" t="n">
-        <v>0.94702</v>
+        <v>0.95</v>
       </c>
       <c r="E51" t="n">
-        <v>0.92276</v>
+        <v>0.97</v>
       </c>
       <c r="F51" t="n">
-        <v>0.91651</v>
+        <v>0.92</v>
       </c>
       <c r="G51" t="n">
-        <v>0.90614</v>
+        <v>0.91</v>
       </c>
       <c r="H51" t="n">
-        <v>0.93125</v>
+        <v>0.93</v>
       </c>
       <c r="I51" t="n">
-        <v>0.96656</v>
+        <v>0.97</v>
       </c>
       <c r="J51" t="n">
-        <v>0.88838</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="52">
@@ -2241,31 +2241,31 @@
         <v>60</v>
       </c>
       <c r="B52" t="n">
-        <v>1.20444</v>
+        <v>1.2</v>
       </c>
       <c r="C52" t="n">
-        <v>1.00378</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>0.92825</v>
+        <v>0.93</v>
       </c>
       <c r="E52" t="n">
-        <v>0.93676</v>
+        <v>0.96</v>
       </c>
       <c r="F52" t="n">
-        <v>0.88383</v>
+        <v>0.88</v>
       </c>
       <c r="G52" t="n">
-        <v>0.89312</v>
+        <v>0.89</v>
       </c>
       <c r="H52" t="n">
-        <v>0.90978</v>
+        <v>0.91</v>
       </c>
       <c r="I52" t="n">
-        <v>0.94985</v>
+        <v>0.95</v>
       </c>
       <c r="J52" t="n">
-        <v>0.88626</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="53">
@@ -2273,31 +2273,31 @@
         <v>61</v>
       </c>
       <c r="B53" t="n">
-        <v>1.20444</v>
+        <v>1.2</v>
       </c>
       <c r="C53" t="n">
-        <v>1.00378</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>0.86968</v>
+        <v>0.87</v>
       </c>
       <c r="E53" t="n">
-        <v>0.90515</v>
+        <v>0.94</v>
       </c>
       <c r="F53" t="n">
-        <v>0.82031</v>
+        <v>0.82</v>
       </c>
       <c r="G53" t="n">
-        <v>0.82789</v>
+        <v>0.83</v>
       </c>
       <c r="H53" t="n">
-        <v>0.87904</v>
+        <v>0.88</v>
       </c>
       <c r="I53" t="n">
-        <v>0.92945</v>
+        <v>0.93</v>
       </c>
       <c r="J53" t="n">
-        <v>0.87949</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="54">
@@ -2305,31 +2305,31 @@
         <v>62</v>
       </c>
       <c r="B54" t="n">
-        <v>1.20212</v>
+        <v>1.2</v>
       </c>
       <c r="C54" t="n">
-        <v>0.92006</v>
+        <v>0.92</v>
       </c>
       <c r="D54" t="n">
-        <v>0.74758</v>
+        <v>0.75</v>
       </c>
       <c r="E54" t="n">
-        <v>0.86741</v>
+        <v>0.93</v>
       </c>
       <c r="F54" t="n">
-        <v>0.7609</v>
+        <v>0.76</v>
       </c>
       <c r="G54" t="n">
-        <v>0.7609</v>
+        <v>0.76</v>
       </c>
       <c r="H54" t="n">
-        <v>0.83406</v>
+        <v>0.83</v>
       </c>
       <c r="I54" t="n">
-        <v>0.88261</v>
+        <v>0.88</v>
       </c>
       <c r="J54" t="n">
-        <v>0.85001</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="55">
@@ -2337,31 +2337,31 @@
         <v>63</v>
       </c>
       <c r="B55" t="n">
-        <v>1.20212</v>
+        <v>1.2</v>
       </c>
       <c r="C55" t="n">
-        <v>0.98708</v>
+        <v>0.99</v>
       </c>
       <c r="D55" t="n">
-        <v>0.67703</v>
+        <v>0.68</v>
       </c>
       <c r="E55" t="n">
-        <v>0.93628</v>
+        <v>0.9</v>
       </c>
       <c r="F55" t="n">
-        <v>0.73264</v>
+        <v>0.73</v>
       </c>
       <c r="G55" t="n">
-        <v>0.7674</v>
+        <v>0.77</v>
       </c>
       <c r="H55" t="n">
-        <v>0.84437</v>
+        <v>0.84</v>
       </c>
       <c r="I55" t="n">
-        <v>0.90862</v>
+        <v>0.91</v>
       </c>
       <c r="J55" t="n">
-        <v>0.8375</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="56">
@@ -2369,31 +2369,31 @@
         <v>64</v>
       </c>
       <c r="B56" t="n">
-        <v>1.20212</v>
+        <v>1.2</v>
       </c>
       <c r="C56" t="n">
-        <v>0.98708</v>
+        <v>0.99</v>
       </c>
       <c r="D56" t="n">
-        <v>0.62576</v>
+        <v>0.63</v>
       </c>
       <c r="E56" t="n">
-        <v>0.96289</v>
+        <v>0.87</v>
       </c>
       <c r="F56" t="n">
-        <v>0.6633</v>
+        <v>0.66</v>
       </c>
       <c r="G56" t="n">
-        <v>0.69304</v>
+        <v>0.69</v>
       </c>
       <c r="H56" t="n">
-        <v>0.83743</v>
+        <v>0.84</v>
       </c>
       <c r="I56" t="n">
-        <v>0.91047</v>
+        <v>0.91</v>
       </c>
       <c r="J56" t="n">
-        <v>0.83492</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="57">
@@ -2401,31 +2401,31 @@
         <v>65</v>
       </c>
       <c r="B57" t="n">
-        <v>0.52868</v>
+        <v>0.53</v>
       </c>
       <c r="C57" t="n">
-        <v>1.06105</v>
+        <v>1.06</v>
       </c>
       <c r="D57" t="n">
-        <v>1.06883</v>
+        <v>1.07</v>
       </c>
       <c r="E57" t="n">
-        <v>1.08733</v>
+        <v>1.1</v>
       </c>
       <c r="F57" t="n">
-        <v>1.05735</v>
+        <v>1.06</v>
       </c>
       <c r="G57" t="n">
-        <v>1.07394</v>
+        <v>1.07</v>
       </c>
       <c r="H57" t="n">
-        <v>1.04651</v>
+        <v>1.05</v>
       </c>
       <c r="I57" t="n">
-        <v>1.06574</v>
+        <v>1.07</v>
       </c>
       <c r="J57" t="n">
-        <v>0.95659</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="58">
@@ -2433,31 +2433,31 @@
         <v>66</v>
       </c>
       <c r="B58" t="n">
-        <v>0.52868</v>
+        <v>0.53</v>
       </c>
       <c r="C58" t="n">
-        <v>1.06105</v>
+        <v>1.06</v>
       </c>
       <c r="D58" t="n">
-        <v>1.09341</v>
+        <v>1.09</v>
       </c>
       <c r="E58" t="n">
-        <v>1.09554</v>
+        <v>1.09</v>
       </c>
       <c r="F58" t="n">
-        <v>1.10702</v>
+        <v>1.11</v>
       </c>
       <c r="G58" t="n">
-        <v>1.02942</v>
+        <v>1.03</v>
       </c>
       <c r="H58" t="n">
-        <v>1.0623</v>
+        <v>1.06</v>
       </c>
       <c r="I58" t="n">
-        <v>1.05708</v>
+        <v>1.06</v>
       </c>
       <c r="J58" t="n">
-        <v>0.89202</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="59">
@@ -2465,31 +2465,31 @@
         <v>67</v>
       </c>
       <c r="B59" t="n">
-        <v>0.5243</v>
+        <v>0.52</v>
       </c>
       <c r="C59" t="n">
-        <v>1.05631</v>
+        <v>1.06</v>
       </c>
       <c r="D59" t="n">
-        <v>1.11894</v>
+        <v>1.12</v>
       </c>
       <c r="E59" t="n">
-        <v>1.12395</v>
+        <v>1.12</v>
       </c>
       <c r="F59" t="n">
-        <v>0.99431</v>
+        <v>0.99</v>
       </c>
       <c r="G59" t="n">
-        <v>1.02884</v>
+        <v>1.03</v>
       </c>
       <c r="H59" t="n">
-        <v>1.04915</v>
+        <v>1.05</v>
       </c>
       <c r="I59" t="n">
-        <v>1.05126</v>
+        <v>1.05</v>
       </c>
       <c r="J59" t="n">
-        <v>0.83525</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="60">
@@ -2497,31 +2497,31 @@
         <v>68</v>
       </c>
       <c r="B60" t="n">
-        <v>0.5243</v>
+        <v>0.52</v>
       </c>
       <c r="C60" t="n">
-        <v>1.03648</v>
+        <v>1.04</v>
       </c>
       <c r="D60" t="n">
-        <v>1.12396</v>
+        <v>1.12</v>
       </c>
       <c r="E60" t="n">
-        <v>1.1065</v>
+        <v>1.11</v>
       </c>
       <c r="F60" t="n">
-        <v>1.206</v>
+        <v>1.21</v>
       </c>
       <c r="G60" t="n">
-        <v>1.13814</v>
+        <v>1.14</v>
       </c>
       <c r="H60" t="n">
-        <v>1.08765</v>
+        <v>1.09</v>
       </c>
       <c r="I60" t="n">
-        <v>1.07716</v>
+        <v>1.08</v>
       </c>
       <c r="J60" t="n">
-        <v>0.97323</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="61">
@@ -2529,31 +2529,31 @@
         <v>69</v>
       </c>
       <c r="B61" t="n">
-        <v>0.5243</v>
+        <v>0.52</v>
       </c>
       <c r="C61" t="n">
-        <v>1.03648</v>
+        <v>1.04</v>
       </c>
       <c r="D61" t="n">
-        <v>1.11885</v>
+        <v>1.12</v>
       </c>
       <c r="E61" t="n">
-        <v>1.109</v>
+        <v>1.14</v>
       </c>
       <c r="F61" t="n">
-        <v>1.16798</v>
+        <v>1.17</v>
       </c>
       <c r="G61" t="n">
-        <v>1.13755</v>
+        <v>1.14</v>
       </c>
       <c r="H61" t="n">
-        <v>1.10668</v>
+        <v>1.11</v>
       </c>
       <c r="I61" t="n">
-        <v>1.06877</v>
+        <v>1.07</v>
       </c>
       <c r="J61" t="n">
-        <v>0.93708</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="62">
@@ -2561,31 +2561,31 @@
         <v>70</v>
       </c>
       <c r="B62" t="n">
-        <v>0.52046</v>
+        <v>0.52</v>
       </c>
       <c r="C62" t="n">
-        <v>1.04646</v>
+        <v>1.05</v>
       </c>
       <c r="D62" t="n">
-        <v>1.07287</v>
+        <v>1.07</v>
       </c>
       <c r="E62" t="n">
-        <v>1.08562</v>
+        <v>1.11</v>
       </c>
       <c r="F62" t="n">
-        <v>1.14432</v>
+        <v>1.14</v>
       </c>
       <c r="G62" t="n">
-        <v>1.09673</v>
+        <v>1.1</v>
       </c>
       <c r="H62" t="n">
-        <v>1.07395</v>
+        <v>1.07</v>
       </c>
       <c r="I62" t="n">
-        <v>1.05443</v>
+        <v>1.05</v>
       </c>
       <c r="J62" t="n">
-        <v>0.89428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="63">
@@ -2593,31 +2593,31 @@
         <v>71</v>
       </c>
       <c r="B63" t="n">
-        <v>0.52046</v>
+        <v>0.52</v>
       </c>
       <c r="C63" t="n">
-        <v>1.02253</v>
+        <v>1.02</v>
       </c>
       <c r="D63" t="n">
-        <v>1.11389</v>
+        <v>1.11</v>
       </c>
       <c r="E63" t="n">
-        <v>1.05639</v>
+        <v>1.05</v>
       </c>
       <c r="F63" t="n">
-        <v>1.0554</v>
+        <v>1.06</v>
       </c>
       <c r="G63" t="n">
-        <v>1.08085</v>
+        <v>1.08</v>
       </c>
       <c r="H63" t="n">
-        <v>1.04437</v>
+        <v>1.04</v>
       </c>
       <c r="I63" t="n">
-        <v>1.07652</v>
+        <v>1.08</v>
       </c>
       <c r="J63" t="n">
-        <v>0.93782</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="64">
@@ -2625,31 +2625,31 @@
         <v>72</v>
       </c>
       <c r="B64" t="n">
-        <v>0.52046</v>
+        <v>0.52</v>
       </c>
       <c r="C64" t="n">
-        <v>1.02253</v>
+        <v>1.02</v>
       </c>
       <c r="D64" t="n">
-        <v>1.13549</v>
+        <v>1.14</v>
       </c>
       <c r="E64" t="n">
-        <v>1.0608</v>
+        <v>1.12</v>
       </c>
       <c r="F64" t="n">
-        <v>1.00343</v>
+        <v>1</v>
       </c>
       <c r="G64" t="n">
-        <v>0.97149</v>
+        <v>0.97</v>
       </c>
       <c r="H64" t="n">
-        <v>1.03679</v>
+        <v>1.04</v>
       </c>
       <c r="I64" t="n">
-        <v>1.07924</v>
+        <v>1.08</v>
       </c>
       <c r="J64" t="n">
-        <v>0.88899</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="65">
@@ -2657,31 +2657,31 @@
         <v>73</v>
       </c>
       <c r="B65" t="n">
-        <v>0.51809</v>
+        <v>0.52</v>
       </c>
       <c r="C65" t="n">
-        <v>0.96503</v>
+        <v>0.97</v>
       </c>
       <c r="D65" t="n">
-        <v>1.09312</v>
+        <v>1.09</v>
       </c>
       <c r="E65" t="n">
-        <v>1.05506</v>
+        <v>1.11</v>
       </c>
       <c r="F65" t="n">
-        <v>0.97417</v>
+        <v>0.97</v>
       </c>
       <c r="G65" t="n">
-        <v>0.91061</v>
+        <v>0.91</v>
       </c>
       <c r="H65" t="n">
-        <v>1.06211</v>
+        <v>1.06</v>
       </c>
       <c r="I65" t="n">
-        <v>1.05967</v>
+        <v>1.06</v>
       </c>
       <c r="J65" t="n">
-        <v>0.83522</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="66">
@@ -2689,31 +2689,31 @@
         <v>74</v>
       </c>
       <c r="B66" t="n">
-        <v>0.51809</v>
+        <v>0.52</v>
       </c>
       <c r="C66" t="n">
-        <v>1.01549</v>
+        <v>1.02</v>
       </c>
       <c r="D66" t="n">
-        <v>1.07013</v>
+        <v>1.07</v>
       </c>
       <c r="E66" t="n">
-        <v>1.07929</v>
+        <v>1.11</v>
       </c>
       <c r="F66" t="n">
-        <v>0.96491</v>
+        <v>0.96</v>
       </c>
       <c r="G66" t="n">
-        <v>0.95461</v>
+        <v>0.95</v>
       </c>
       <c r="H66" t="n">
-        <v>1.01574</v>
+        <v>1.02</v>
       </c>
       <c r="I66" t="n">
-        <v>1.06868</v>
+        <v>1.07</v>
       </c>
       <c r="J66" t="n">
-        <v>0.89515</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="67">
@@ -2721,31 +2721,31 @@
         <v>75</v>
       </c>
       <c r="B67" t="n">
-        <v>0.51809</v>
+        <v>0.52</v>
       </c>
       <c r="C67" t="n">
-        <v>1.01549</v>
+        <v>1.02</v>
       </c>
       <c r="D67" t="n">
-        <v>1.05209</v>
+        <v>1.05</v>
       </c>
       <c r="E67" t="n">
-        <v>1.09081</v>
+        <v>1.14</v>
       </c>
       <c r="F67" t="n">
-        <v>1.02388</v>
+        <v>1.02</v>
       </c>
       <c r="G67" t="n">
-        <v>1.02964</v>
+        <v>1.03</v>
       </c>
       <c r="H67" t="n">
-        <v>1.02874</v>
+        <v>1.03</v>
       </c>
       <c r="I67" t="n">
-        <v>1.08223</v>
+        <v>1.08</v>
       </c>
       <c r="J67" t="n">
-        <v>0.88754</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="68">
@@ -2753,31 +2753,31 @@
         <v>76</v>
       </c>
       <c r="B68" t="n">
-        <v>0.39244</v>
+        <v>0.39</v>
       </c>
       <c r="C68" t="n">
-        <v>1.03175</v>
+        <v>1.03</v>
       </c>
       <c r="D68" t="n">
-        <v>1.06102</v>
+        <v>1.06</v>
       </c>
       <c r="E68" t="n">
-        <v>1.08335</v>
+        <v>1.09</v>
       </c>
       <c r="F68" t="n">
-        <v>0.99206</v>
+        <v>0.99</v>
       </c>
       <c r="G68" t="n">
-        <v>1.02103</v>
+        <v>1.02</v>
       </c>
       <c r="H68" t="n">
-        <v>1.05037</v>
+        <v>1.05</v>
       </c>
       <c r="I68" t="n">
-        <v>1.06865</v>
+        <v>1.07</v>
       </c>
       <c r="J68" t="n">
-        <v>1.13635</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="69">
@@ -2785,31 +2785,31 @@
         <v>77</v>
       </c>
       <c r="B69" t="n">
-        <v>0.39244</v>
+        <v>0.39</v>
       </c>
       <c r="C69" t="n">
-        <v>1.03175</v>
+        <v>1.03</v>
       </c>
       <c r="D69" t="n">
-        <v>1.05395</v>
+        <v>1.05</v>
       </c>
       <c r="E69" t="n">
-        <v>1.07826</v>
+        <v>1.11</v>
       </c>
       <c r="F69" t="n">
-        <v>1.00827</v>
+        <v>1.01</v>
       </c>
       <c r="G69" t="n">
-        <v>1.03109</v>
+        <v>1.03</v>
       </c>
       <c r="H69" t="n">
-        <v>1.0616</v>
+        <v>1.06</v>
       </c>
       <c r="I69" t="n">
-        <v>1.03855</v>
+        <v>1.04</v>
       </c>
       <c r="J69" t="n">
-        <v>1.09713</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="70">
@@ -2817,31 +2817,31 @@
         <v>78</v>
       </c>
       <c r="B70" t="n">
-        <v>0.39047</v>
+        <v>0.39</v>
       </c>
       <c r="C70" t="n">
-        <v>1.02464</v>
+        <v>1.02</v>
       </c>
       <c r="D70" t="n">
-        <v>1.06685</v>
+        <v>1.07</v>
       </c>
       <c r="E70" t="n">
-        <v>1.08239</v>
+        <v>1.12</v>
       </c>
       <c r="F70" t="n">
-        <v>1.05844</v>
+        <v>1.06</v>
       </c>
       <c r="G70" t="n">
-        <v>1.03464</v>
+        <v>1.03</v>
       </c>
       <c r="H70" t="n">
-        <v>1.03799</v>
+        <v>1.04</v>
       </c>
       <c r="I70" t="n">
-        <v>1.01894</v>
+        <v>1.02</v>
       </c>
       <c r="J70" t="n">
-        <v>1.04481</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="71">
@@ -2849,31 +2849,31 @@
         <v>79</v>
       </c>
       <c r="B71" t="n">
-        <v>0.39047</v>
+        <v>0.39</v>
       </c>
       <c r="C71" t="n">
-        <v>1.0348</v>
+        <v>1.03</v>
       </c>
       <c r="D71" t="n">
-        <v>1.0634</v>
+        <v>1.06</v>
       </c>
       <c r="E71" t="n">
-        <v>1.05424</v>
+        <v>1.09</v>
       </c>
       <c r="F71" t="n">
-        <v>1.05734</v>
+        <v>1.06</v>
       </c>
       <c r="G71" t="n">
-        <v>1.07156</v>
+        <v>1.07</v>
       </c>
       <c r="H71" t="n">
-        <v>1.05583</v>
+        <v>1.06</v>
       </c>
       <c r="I71" t="n">
-        <v>1.03985</v>
+        <v>1.04</v>
       </c>
       <c r="J71" t="n">
-        <v>1.03846</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="72">
@@ -2881,31 +2881,31 @@
         <v>80</v>
       </c>
       <c r="B72" t="n">
-        <v>0.39047</v>
+        <v>0.39</v>
       </c>
       <c r="C72" t="n">
-        <v>1.0348</v>
+        <v>1.03</v>
       </c>
       <c r="D72" t="n">
-        <v>1.06133</v>
+        <v>1.06</v>
       </c>
       <c r="E72" t="n">
-        <v>1.06007</v>
+        <v>1.11</v>
       </c>
       <c r="F72" t="n">
-        <v>1.14835</v>
+        <v>1.15</v>
       </c>
       <c r="G72" t="n">
-        <v>1.15803</v>
+        <v>1.16</v>
       </c>
       <c r="H72" t="n">
-        <v>1.07658</v>
+        <v>1.08</v>
       </c>
       <c r="I72" t="n">
-        <v>1.02224</v>
+        <v>1.02</v>
       </c>
       <c r="J72" t="n">
-        <v>1.04776</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="73">
@@ -2913,31 +2913,31 @@
         <v>81</v>
       </c>
       <c r="B73" t="n">
-        <v>0.3886</v>
+        <v>0.39</v>
       </c>
       <c r="C73" t="n">
-        <v>1.0263</v>
+        <v>1.03</v>
       </c>
       <c r="D73" t="n">
-        <v>1.05654</v>
+        <v>1.06</v>
       </c>
       <c r="E73" t="n">
-        <v>1.03763</v>
+        <v>1.12</v>
       </c>
       <c r="F73" t="n">
-        <v>1.21189</v>
+        <v>1.21</v>
       </c>
       <c r="G73" t="n">
-        <v>1.21954</v>
+        <v>1.22</v>
       </c>
       <c r="H73" t="n">
-        <v>1.00789</v>
+        <v>1.01</v>
       </c>
       <c r="I73" t="n">
-        <v>1.02499</v>
+        <v>1.02</v>
       </c>
       <c r="J73" t="n">
-        <v>1.06109</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="74">
@@ -2945,31 +2945,31 @@
         <v>82</v>
       </c>
       <c r="B74" t="n">
-        <v>0.3886</v>
+        <v>0.39</v>
       </c>
       <c r="C74" t="n">
-        <v>1.02767</v>
+        <v>1.03</v>
       </c>
       <c r="D74" t="n">
-        <v>1.05149</v>
+        <v>1.05</v>
       </c>
       <c r="E74" t="n">
-        <v>1.02889</v>
+        <v>1.08</v>
       </c>
       <c r="F74" t="n">
-        <v>1.0414</v>
+        <v>1.04</v>
       </c>
       <c r="G74" t="n">
-        <v>1.03407</v>
+        <v>1.03</v>
       </c>
       <c r="H74" t="n">
-        <v>1.00137</v>
+        <v>1</v>
       </c>
       <c r="I74" t="n">
-        <v>1.05294</v>
+        <v>1.05</v>
       </c>
       <c r="J74" t="n">
-        <v>0.99458</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="75">
@@ -2977,31 +2977,31 @@
         <v>83</v>
       </c>
       <c r="B75" t="n">
-        <v>0.3886</v>
+        <v>0.39</v>
       </c>
       <c r="C75" t="n">
-        <v>1.02767</v>
+        <v>1.03</v>
       </c>
       <c r="D75" t="n">
-        <v>1.06344</v>
+        <v>1.06</v>
       </c>
       <c r="E75" t="n">
-        <v>1.02703</v>
+        <v>1.11</v>
       </c>
       <c r="F75" t="n">
-        <v>1.21662</v>
+        <v>1.22</v>
       </c>
       <c r="G75" t="n">
-        <v>1.15852</v>
+        <v>1.16</v>
       </c>
       <c r="H75" t="n">
-        <v>0.99581</v>
+        <v>1</v>
       </c>
       <c r="I75" t="n">
-        <v>1.01593</v>
+        <v>1.02</v>
       </c>
       <c r="J75" t="n">
-        <v>0.98131</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="76">
@@ -3009,31 +3009,31 @@
         <v>84</v>
       </c>
       <c r="B76" t="n">
-        <v>0.38675</v>
+        <v>0.39</v>
       </c>
       <c r="C76" t="n">
-        <v>1.08151</v>
+        <v>1.08</v>
       </c>
       <c r="D76" t="n">
-        <v>1.07481</v>
+        <v>1.07</v>
       </c>
       <c r="E76" t="n">
-        <v>1.02376</v>
+        <v>1.12</v>
       </c>
       <c r="F76" t="n">
-        <v>1.10617</v>
+        <v>1.11</v>
       </c>
       <c r="G76" t="n">
-        <v>1.15899</v>
+        <v>1.16</v>
       </c>
       <c r="H76" t="n">
-        <v>0.99293</v>
+        <v>0.99</v>
       </c>
       <c r="I76" t="n">
-        <v>1.01257</v>
+        <v>1.01</v>
       </c>
       <c r="J76" t="n">
-        <v>1.01539</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="77">
@@ -3041,31 +3041,31 @@
         <v>85</v>
       </c>
       <c r="B77" t="n">
-        <v>0.38675</v>
+        <v>0.39</v>
       </c>
       <c r="C77" t="n">
-        <v>1.03254</v>
+        <v>1.03</v>
       </c>
       <c r="D77" t="n">
-        <v>1.06093</v>
+        <v>1.06</v>
       </c>
       <c r="E77" t="n">
-        <v>0.9975</v>
+        <v>1.1</v>
       </c>
       <c r="F77" t="n">
-        <v>1.06983</v>
+        <v>1.07</v>
       </c>
       <c r="G77" t="n">
-        <v>1.04996</v>
+        <v>1.05</v>
       </c>
       <c r="H77" t="n">
-        <v>1.02741</v>
+        <v>1.03</v>
       </c>
       <c r="I77" t="n">
-        <v>1.04186</v>
+        <v>1.04</v>
       </c>
       <c r="J77" t="n">
-        <v>1.04366</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="78">
@@ -3073,31 +3073,31 @@
         <v>86</v>
       </c>
       <c r="B78" t="n">
-        <v>0.38675</v>
+        <v>0.39</v>
       </c>
       <c r="C78" t="n">
-        <v>1.03254</v>
+        <v>1.03</v>
       </c>
       <c r="D78" t="n">
-        <v>1.01256</v>
+        <v>1.01</v>
       </c>
       <c r="E78" t="n">
-        <v>0.95477</v>
+        <v>1.13</v>
       </c>
       <c r="F78" t="n">
-        <v>1.10701</v>
+        <v>1.11</v>
       </c>
       <c r="G78" t="n">
-        <v>1.21697</v>
+        <v>1.22</v>
       </c>
       <c r="H78" t="n">
-        <v>1.00947</v>
+        <v>1.01</v>
       </c>
       <c r="I78" t="n">
-        <v>1.01483</v>
+        <v>1.01</v>
       </c>
       <c r="J78" t="n">
-        <v>1.01229</v>
+        <v>1.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>